<commit_message>
Added check_in/add_new methods and started check_out
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Condensed Inventory" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Expanded Inventory" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Condensed Inventory" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Expanded Inventory" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>wine_id</t>
   </si>
@@ -78,6 +78,27 @@
     <t>Standard (750 mL)</t>
   </si>
   <si>
+    <t>Syrah</t>
+  </si>
+  <si>
+    <t>$35</t>
+  </si>
+  <si>
+    <t>Turly</t>
+  </si>
+  <si>
+    <t>Zinfandel</t>
+  </si>
+  <si>
+    <t>$40</t>
+  </si>
+  <si>
+    <t>$25</t>
+  </si>
+  <si>
+    <t>Young vines</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
@@ -97,6 +118,18 @@
   </si>
   <si>
     <t>2019-01-15 16:16:52</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>2019-01-22 16:35:03</t>
+  </si>
+  <si>
+    <t>2019-01-22 17:49:41</t>
+  </si>
+  <si>
+    <t>2019-01-22 17:53:58</t>
   </si>
 </sst>
 </file>
@@ -432,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +546,73 @@
         <v>19</v>
       </c>
       <c r="M2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2014</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2011</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -527,7 +627,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,13 +673,13 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="N1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="O1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -614,10 +714,10 @@
         <v>19</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -652,10 +752,121 @@
         <v>19</v>
       </c>
       <c r="M3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2014</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2011</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
         <v>25</v>
       </c>
-      <c r="N3" t="s">
+      <c r="K5" t="s">
         <v>26</v>
+      </c>
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2011</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>